<commit_message>
Confirmed diftool works using Beyond Compare 3 ('bc3')
</commit_message>
<xml_diff>
--- a/ideas/OLR/xls_standard_input_IDEAS.xlsx
+++ b/ideas/OLR/xls_standard_input_IDEAS.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7787" uniqueCount="1967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7787" uniqueCount="1968">
   <si>
     <t>text</t>
   </si>
@@ -6194,6 +6194,9 @@
   </si>
   <si>
     <t>see_if_it_shows_up.pdf</t>
+  </si>
+  <si>
+    <t>Some guy</t>
   </si>
 </sst>
 </file>
@@ -7230,10 +7233,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7419,11 +7422,11 @@
       <c r="C4" s="18" t="s">
         <v>1966</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>0</v>
-      </c>
       <c r="G4" s="18" t="s">
         <v>1965</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>1967</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>